<commit_message>
create Data provider class with test example
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Interview Preparation\JokerFrameWork\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C646B0AB-6D0C-4E4C-A643-DBAC4DD6C109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6694FA-6D93-4203-9FA4-E44FA18C7392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
   <si>
     <t>userNames</t>
   </si>
@@ -34,15 +37,6 @@
   </si>
   <si>
     <t>standard_user</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
@@ -373,8 +367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,31 +390,151 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AC8853-66C1-45FB-B51D-9E27C550408E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1531DCB3-BDF1-4BEF-96B9-4A66D44BCE56}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6873C8-8F44-411B-914A-7CB9A78DC9AB}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>